<commit_message>
Last commit, thx for the project!
</commit_message>
<xml_diff>
--- a/Datasets_Audios_Medicos/wer/resultados_wer.xlsx
+++ b/Datasets_Audios_Medicos/wer/resultados_wer.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,25 +442,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Azure</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>GCP</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Gemini</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>GPT4o</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Duração (s)</t>
         </is>
@@ -474,25 +479,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>16.67%</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>25.0%</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>8.33%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>16.67%</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>9</v>
       </c>
     </row>
@@ -514,16 +524,21 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>18.18%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>5328</v>
+      <c r="G3" t="n">
+        <v>5.33</v>
       </c>
     </row>
     <row r="4">
@@ -544,16 +559,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>16.67%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>5868</v>
+      <c r="G4" t="n">
+        <v>5.87</v>
       </c>
     </row>
     <row r="5">
@@ -569,21 +589,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>66.67%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>88.89%</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>77.78%</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>311.11%</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>7416</v>
+      <c r="G5" t="n">
+        <v>7.42</v>
       </c>
     </row>
     <row r="6">
@@ -599,21 +624,26 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>11.11%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>0.0%</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>55.56%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>111.11%</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>7956</v>
+      <c r="G6" t="n">
+        <v>7.96</v>
       </c>
     </row>
     <row r="7">
@@ -624,26 +654,31 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>42.86%</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>28.57%</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>57.14%</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>42.86%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>300.0%</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>5868</v>
+      <c r="G7" t="n">
+        <v>5.87</v>
       </c>
     </row>
     <row r="8">
@@ -654,26 +689,31 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>8.33%</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>25.0%</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>8.33%</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>8.33%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>25.0%</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>7740</v>
+      <c r="G8" t="n">
+        <v>7.74</v>
       </c>
     </row>
     <row r="9">
@@ -684,25 +724,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>13.59%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>9.32%</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>17.09%</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>16.89%</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>9.32%</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>190.2</v>
       </c>
     </row>
@@ -714,25 +759,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>17.5%</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>18.44%</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>21.56%</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>33.12%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>22.81%</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>130.4</v>
       </c>
     </row>
@@ -744,25 +794,30 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>28.15%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>26.49%</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>24.17%</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>30.79%</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>55.63%</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>93</v>
       </c>
     </row>
@@ -774,25 +829,30 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>66.67%</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>49.21%</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>42.06%</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>38.1%</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>48.5</v>
       </c>
     </row>
@@ -804,25 +864,30 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>8.98%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>10.78%</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>10.58%</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>18.76%</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>8.78%</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>174.8</v>
       </c>
     </row>
@@ -834,21 +899,30 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>36.1%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>29.01%</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>39.9%</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>44.4%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>75.36%</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
         <v>583.4</v>
       </c>
     </row>
@@ -860,21 +934,30 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>2.27%</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>1.13%</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>2.55%</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>11.33%</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1.42%</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>191.8</v>
       </c>
     </row>
@@ -886,21 +969,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>3.71%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>2.74%</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>6.29%</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>8.39%</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2.58%</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
         <v>285.8</v>
       </c>
     </row>
@@ -912,21 +1004,30 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>6.29%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>7.63%</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>9.13%</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>16.32%</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>5.24%</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
         <v>253.4</v>
       </c>
     </row>
@@ -938,21 +1039,30 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>26.73%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>7.49%</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>7.78%</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>15.42%</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2.94%</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
         <v>278.8</v>
       </c>
     </row>
@@ -964,22 +1074,31 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>12.59%</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>15.56%</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>29.47%</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>14.04%</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>530000</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>16.08%</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>530</v>
       </c>
     </row>
     <row r="20">
@@ -995,16 +1114,25 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>17.86%</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>16.07%</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>21.43%</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="n">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>16.07%</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
         <v>29.9</v>
       </c>
     </row>
@@ -1016,21 +1144,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>13.33%</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>11.85%</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>10.37%</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>9.63%</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1.48%</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
         <v>65.59999999999999</v>
       </c>
     </row>
@@ -1042,22 +1179,31 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>26.09%</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>30.43%</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>30.43%</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>47.83%</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>8000</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>8.7%</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -1068,22 +1214,31 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>65.12%</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>51.16%</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>41.86%</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>67.44%</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>19000</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>65.12%</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="24">
@@ -1094,22 +1249,31 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>5.95%</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>9.73%</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>9.73%</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>10.27%</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>43000</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>5.41%</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1149,10 +1313,8 @@
           <t>AWS</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B2" t="n">
+        <v>18.35</v>
       </c>
     </row>
     <row r="3">
@@ -1162,7 +1324,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16.9</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="4">
@@ -1172,7 +1334,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>28.29</v>
+        <v>20.76</v>
       </c>
     </row>
     <row r="5">
@@ -1182,7 +1344,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.33</v>
+        <v>22.47</v>
       </c>
     </row>
     <row r="6">
@@ -1192,7 +1354,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>144.2</v>
+        <v>25.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>